<commit_message>
Added new data from another group for HVO60
</commit_message>
<xml_diff>
--- a/ExampleDataSet/Data/Session2.xlsx
+++ b/ExampleDataSet/Data/Session2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/j_hu3_student_tue_nl/Documents/Desktop/Sustainable fuels git/ExampleDataSet/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{F77490D0-0507-4D8C-91E0-10AC8A80EAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94F8A655-97BD-4EC5-BF5E-D833ECFDD7DE}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{F77490D0-0507-4D8C-91E0-10AC8A80EAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACAC92CF-135A-47D5-BCE3-58737AABEEF2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C018F7D-E519-4136-B5E8-DCCAC3EF0FC5}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{5C018F7D-E519-4136-B5E8-DCCAC3EF0FC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>CO [%]</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>Session 2 results</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -154,6 +158,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8587CCB6-2983-41F7-8455-B97F90EC9C03}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,4 +732,259 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91E181A-A8AE-4D92-9DE3-6BB0DB932161}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>335</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>14.42</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>360</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F23" s="3">
+        <v>14.45</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>385</v>
+      </c>
+      <c r="E24" s="3">
+        <v>45</v>
+      </c>
+      <c r="F24" s="3">
+        <v>14.44</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>424</v>
+      </c>
+      <c r="E25" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F25" s="3">
+        <v>14.4</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>477</v>
+      </c>
+      <c r="E26" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F26" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F27" s="3">
+        <v>14.45</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>20</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F28" s="3">
+        <v>14.38</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>